<commit_message>
completed summary dataframe and timings
</commit_message>
<xml_diff>
--- a/CourseProposal/json_output/assessment_dataframe.xlsx
+++ b/CourseProposal/json_output/assessment_dataframe.xlsx
@@ -58,55 +58,55 @@
     <t>Written Exam</t>
   </si>
   <si>
-    <t>For A1: Analyzing release components is evaluated through practical tasks where trainees identify and examine elements.
+    <t>Practical exercises provide a direct demonstration of the ability to analyze release components. Assessing the practical application of identifying and understanding the different components of a release.
 A1: Analyse release components (ICT-DIT-3014-1.1)</t>
   </si>
   <si>
-    <t>For A2: Coordination is assessed via practical tasks where trainees must communicate during simulated release scheduling.
+    <t>Practical exercises simulate real-world scenarios requiring coordination. Assessing the ability to communicate effectively and align release activities with stakeholders' needs and timelines.
 A2: Coordinate with relevant stakeholders on release scheduling to align release processes and procedures (ICT-DIT-3014-1.1)</t>
   </si>
   <si>
-    <t>For K1: Practical exercises directly assess understanding of script/tool types and usage for integration and deployment.
+    <t>Practical exercises assess the application of knowledge regarding scripts and tools, and their usage in software integration and deployment. It tests understanding of when and how to use specific tools.
 K1: Types and usage of scripts and tools for integrating and deploying software products (ICT-DIT-3014-1.1)</t>
   </si>
   <si>
-    <t>For A3: Practical exercises require trainees to choose appropriate scripts/tools, assessing selection skills.
+    <t>Practical assessment demonstrates the ability to choose appropriate scripts and tools. Focusing on effectiveness and suitability for specific integration and deployment tasks, evaluating selection skills.
 A3: Select appropriate scripts and tools for integrating and deploying software products (ICT-DIT-3014-1.1)</t>
   </si>
   <si>
-    <t>For K2: Software configuration procedures are directly assessed in practical exercises, where trainees configure software.
+    <t>Practical application tests the understanding of software configuration procedures by requiring candidates to execute these procedures, showing they understand each step's purpose and sequence.
 K2: Software configuration procedures (ICT-DIT-3014-1.1)</t>
   </si>
   <si>
-    <t>For K3: Configuration test knowledge is assessed through identifying purposes in practical exercises.
+    <t>Configuration tests are included to check the candidate knows the configuration tests performed, and their purpose in ensuring the reliability and stability of the software product.
 K3: Configuration tests and their purposes (ICT-DIT-3014-1.1)</t>
   </si>
   <si>
-    <t>For A4: Software configuration skills are evaluated directly through hands-on configuration tasks in practicals.
+    <t>Practical exercises test the ability to configure software. It assesses the ability to translate theoretical knowledge into practical skills in diverse platform configurations.
 A4: Configure software products to integrate and deploy software releases to various platforms (ICT-DIT-3014-1.1)</t>
   </si>
   <si>
-    <t>For A5: Practical exercises directly assess executing config tests during hands-on activities.
+    <t>Practical activities demonstrate competency in executing configuration tests. Assessing the ability to follow procedures accurately and efficiently, while understanding the expected outcomes.
 A5: Execute configuration tests on platform specific versions of software products in line with testing procedures (ICT-DIT-3014-1.1)</t>
   </si>
   <si>
-    <t>For K4: Interpreting configuration test results is assessed by analyzing output during practical exercises.
+    <t>Practical activities ensures the candidate can determine the outcome, issues or successes of testing procedures, and ensures the software is functional after configuration tests.
 K4: Interpretation of configuration test results (ICT-DIT-3014-1.1)</t>
   </si>
   <si>
-    <t>For A6: Practical work and configuration test results are analysed to diagnose issues surfaced from configuration testing
+    <t>Practical tests involve identifying the cause and remedy to issues, which allows for assessment of their ability to diagnose effectively. The configuration allows a setting for practical investigation.
 A6: Diagnose issues surfaced from configuration testing (ICT-DIT-3014-1.1)</t>
   </si>
   <si>
-    <t>For K5: Practical tasks will indirectly show knowledge of deployment process elements when trainees perform them.
+    <t>The practical element ensures the candidate understands the software configuration and deployment process, and they have appropriate knowledge to perform actions that will be tested in action.
 K5: Elements of the software configuration and deployment process (ICT-DIT-3014-1.1)</t>
   </si>
   <si>
-    <t>For A7: Improvements are identified by trainees during exercises, assessing their analytical and improvement skills.
+    <t>Practical implementation allows for the ability to determine improvements from the outcome of testing, and their experience, which allows for better modification of software code.
 A7: Identify potential improvements and modifications to the software configuration and deployment process or the software code (ICT-DIT-3014-1.1)</t>
   </si>
   <si>
-    <t>For A8: Implementing modifications is directly assessed by evaluating successful changes made during practicals.
+    <t>The practical element ensures the candidate can properly modify platform-specific software products and processes, while retaining previous functionality and applying improvements.
 A8: Implement modifications to platform-specific software products and processes (ICT-DIT-3014-1.1)</t>
   </si>
 </sst>
@@ -499,7 +499,7 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -519,7 +519,7 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -539,7 +539,7 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -579,7 +579,7 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -599,7 +599,7 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -659,7 +659,7 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -699,7 +699,7 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D12">
         <v>1</v>

</xml_diff>

<commit_message>
added test and fixed agents response to fit new excel format
</commit_message>
<xml_diff>
--- a/CourseProposal/json_output/assessment_dataframe.xlsx
+++ b/CourseProposal/json_output/assessment_dataframe.xlsx
@@ -487,7 +487,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>The candidate will answer questions on creative principles and storytelling in AI-generated text prompts to assess understanding.
+          <t>The candidate will describe creative principles and storytelling in AI-generated text prompts in a Written Exam.
 K9: Creative principles and storytelling in AI generated text prompts (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -514,7 +514,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>The candidate will respond to questions on basic AI algorithms and models used in script/text generation to demonstrate knowledge.
+          <t>The candidate will explain basic AI algorithms and models used in script/text generation in a Written Exam.
 K10: Basic AI algorithms and models used in script/text generation (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -541,7 +541,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>The candidate will incorporate unique creative principles and storytelling elements into AI-generated story ideas during a practical exam.
+          <t>The candidate will incorporate unique creative principles into AI-generated story ideas in a Practical Exam.
 A8: Incorporate unique creative principles and storytelling elements into AI-generated story ideas to avoid generic replication (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -568,7 +568,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>The candidate will use AI-generated text techniques and methodologies to develop script elements in a practical exam.
+          <t>The candidate will use AI-generated text techniques to develop script elements in a Practical Exam.
 A5: Use AI-generated text techniques and methodologies to develop script elements (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -595,7 +595,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>The candidate will respond to a series of short answer questions related to AI-generated script ideation techniques for world-building, storyline and character development, scenario iterations.
+          <t>The candidate will respond to a series of short answer questions related to AI-generated script ideation techniques for world-building, storyline, and character development in a Written Exam.
 K1: AI-generated script ideation techniques for world-building, storyline and character development, scenario iterations (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -622,7 +622,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>The candidate will identify key terms and themes for input into Gen AI platform to ideate and iterate story elements in a practical exam.
+          <t>The candidate will identify key terms and themes for input into Gen AI platform in a Practical Exam.
 A7: Identify key terms and themes for input into Gen AI platform to ideate and iterate story elements for incorporation into text prompts (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -649,7 +649,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>The candidate will answer questions on Gen AI tool limitations and solutions to assess their knowledge.
+          <t>The candidate will explain Gen AI tool limitations and solutions in a Written Exam.
 K3: Gen AI tool limitations and solutions (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -676,7 +676,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>The candidate will apply and adjust relevant prompts in the generative process to improve iterations during a practical exam.
+          <t>The candidate will apply and adjust prompts in the generative process to improve iterations in a Practical Exam.
 A6: Apply and adjust relevant prompts in the generative process to improve iterations (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -703,7 +703,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>The candidate will respond to questions on basic NLP techniques and tools relevant to AI text generation to demonstrate knowledge.
+          <t>The candidate will explain basic NLP techniques and tools relevant to AI Text generation in a Written Exam.
 K8: Basic Natural Language Processing (NLP) techniques and tools relevant to AI Text generation (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -730,7 +730,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>The candidate will utilize NLP techniques and tools to enhance the quality and effectiveness of AI-generated story elements in a practical exam.
+          <t>The candidate will utilize NLP techniques and tools to enhance AI-generated story elements in a Practical Exam.
 A2: Utilise NLP techniques and tools to enhance the quality and effectiveness of AI-generated story elements (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -757,7 +757,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>The candidate will respond to questions about AI tools for script analysis and market research to demonstrate knowledge.
+          <t>The candidate will describe AI tools for script analysis and market research in a Written Exam.
 K6: AI tools for script analysis and market research (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -784,7 +784,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>The candidate will filter and script-edit Gen-AI output in a practical exam to demonstrate their skills.
+          <t>The candidate will filter and script-edit Gen-AI output in a Practical Exam.
 A4: Filter and Script-edit Gen-AI output (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -811,7 +811,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>The candidate will answer questions on Gen AI and ethics awareness to assess their understanding.
+          <t>The candidate will discuss Gen AI and Ethics awareness in a Written Exam.
 K7: Gen AI and Ethics awareness (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -838,7 +838,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>The candidate will answer questions on best practices to minimize plagiarism risk to show understanding.
+          <t>The candidate will discuss best practices to minimize plagiarism risk in a Written Exam.
 K5: Best Practices to minimise plagiarism risk (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -865,7 +865,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>The candidate will apply ethical considerations in the selection of prompts and reference usage during a practical exam.
+          <t>The candidate will apply ethical considerations in prompt selection and reference usage in a Practical Exam.
 A3: Apply ethical considerations in the selection of prompts and reference usage (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -892,7 +892,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>The candidate will explain awareness and correction of bias in LLMs training data reproduced in output through written responses.
+          <t>The candidate will demonstrate awareness and correction of bias in LLMs training data in a Written Exam.
 K4: Awareness and correction of bias in LLMs training data reproduced in output (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -919,7 +919,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>The candidate will perform a practical exercise on analyzing AI output for bias and taking corrective steps and submit their analysis.
+          <t>The candidate will perform a practical exercise on analyzing AI output for bias and submit corrective steps in a Practical Exam.
 A1: Analyse AI output for bias and taking corrective steps (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -946,7 +946,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>The candidate will respond to questions about copyright law covering Gen AI usage to demonstrate understanding.
+          <t>The candidate will answer questions on copyright law covering Gen AI usage in a Written Exam.
 K2: Copyright law covering Gen AI usage (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -973,7 +973,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>The candidate will identify copyright risk in Gen-AI production and avoid copyright infringement in a practical exam.
+          <t>The candidate will identify copyright risk in Gen-AI production and avoid infringement in a Practical Exam.
 A9: Identify copyright risk in Gen-AI production and avoid copyright infringement (MED-MED-3004-1.1)</t>
         </is>
       </c>

</xml_diff>